<commit_message>
Update updated kobo and loa
</commit_message>
<xml_diff>
--- a/data-raw/loa.xlsx
+++ b/data-raw/loa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guillaume.noblet\Documents\GitHub\humind.data\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C3F067-92D9-46BD-ABCC-1E406E952484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2460203-E1E7-4670-9489-8D0CBE82D0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_frame" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="update_choices" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">update_choices!$A$1:$H$138</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">update_survey!$A$1:$F$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="746">
   <si>
     <t>admin1</t>
   </si>
@@ -5800,9 +5801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -8147,6 +8148,9 @@
       <c r="E90" s="15" t="s">
         <v>330</v>
       </c>
+      <c r="F90" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="G90" s="15" t="s">
         <v>730</v>
       </c>
@@ -8169,6 +8173,9 @@
       </c>
       <c r="E91" s="15" t="s">
         <v>333</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="G91" s="15" t="s">
         <v>730</v>
@@ -8582,9 +8589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:A34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -10234,6 +10241,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H138" xr:uid="{00000000-0001-0000-0600-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>